<commit_message>
improved weighing function, updated vocab list
</commit_message>
<xml_diff>
--- a/vocab.xlsx
+++ b/vocab.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="170">
   <si>
     <t>text</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Strangulation </t>
   </si>
   <si>
-    <t>Initial suspect was not guilty.</t>
+    <t>Initial suspect was not guilty</t>
   </si>
   <si>
     <t xml:space="preserve">Interrogation </t>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Autopsy </t>
   </si>
   <si>
-    <t xml:space="preserve">“Maximum sentence” </t>
+    <t>Sentencing</t>
   </si>
   <si>
     <t>Suspect’s story changes</t>
@@ -64,7 +64,7 @@
     <t>Evidence bags</t>
   </si>
   <si>
-    <t xml:space="preserve">Crime scene photograph </t>
+    <t>Crime scene photograph or video</t>
   </si>
   <si>
     <t>"Thanks to forensic science...."</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Lands and grooves </t>
   </si>
   <si>
-    <t xml:space="preserve">Rape </t>
+    <t>Rape / sexual assault</t>
   </si>
   <si>
     <t xml:space="preserve">Security camera footage </t>
@@ -196,7 +196,7 @@
     <t xml:space="preserve">Valuables left behind </t>
   </si>
   <si>
-    <t xml:space="preserve">Composite artist makes a sketch </t>
+    <t xml:space="preserve">Composite artist sketch </t>
   </si>
   <si>
     <t xml:space="preserve">Dental identification </t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">Rigor mortis </t>
   </si>
   <si>
-    <t xml:space="preserve">Local journalist interviewed </t>
+    <t>Local journalist</t>
   </si>
   <si>
     <t xml:space="preserve">Witness testimony </t>
@@ -217,7 +217,7 @@
     <t xml:space="preserve">Clothing discarded </t>
   </si>
   <si>
-    <t xml:space="preserve">Clean up job </t>
+    <t xml:space="preserve">Clean-up job </t>
   </si>
   <si>
     <t xml:space="preserve">Microscope analysis </t>
@@ -241,7 +241,7 @@
     <t xml:space="preserve">Poison timeline determined by hair </t>
   </si>
   <si>
-    <t xml:space="preserve">“Literally wrote the book on tire impression evidence” </t>
+    <t xml:space="preserve">“Literally wrote the book on ________” </t>
   </si>
   <si>
     <t xml:space="preserve">Gunshot residue on spouse’s hands but not victim’s hands </t>
@@ -262,7 +262,7 @@
     <t xml:space="preserve">Munchausen syndrome by proxy </t>
   </si>
   <si>
-    <t xml:space="preserve">Stockhold syndrome </t>
+    <t xml:space="preserve">Stockholm syndrome </t>
   </si>
   <si>
     <t xml:space="preserve">Pregnant woman murdered </t>
@@ -337,7 +337,7 @@
     <t>Rental car</t>
   </si>
   <si>
-    <t xml:space="preserve">“String of murders” </t>
+    <t>“String of murders (or rapes)"</t>
   </si>
   <si>
     <t xml:space="preserve">Ligature marks </t>
@@ -403,7 +403,7 @@
     <t>Perpetrator gives an interview</t>
   </si>
   <si>
-    <t>A vehicle is found and searched</t>
+    <t>A vehicle is found and/or searched</t>
   </si>
   <si>
     <t>Local politician</t>
@@ -418,7 +418,7 @@
     <t>"Closure"</t>
   </si>
   <si>
-    <t>Argument overheard</t>
+    <t xml:space="preserve">Argument </t>
   </si>
   <si>
     <t>History of violence</t>
@@ -448,7 +448,7 @@
     <t>Rifle</t>
   </si>
   <si>
-    <t>caliber of bullet / ballistics</t>
+    <t>Caliber of bullet / ballistics</t>
   </si>
   <si>
     <t>Document examiner</t>
@@ -473,6 +473,54 @@
   </si>
   <si>
     <t>Snitch</t>
+  </si>
+  <si>
+    <t>Hair analysis</t>
+  </si>
+  <si>
+    <t>Cop with mustache</t>
+  </si>
+  <si>
+    <t>Tire impressions</t>
+  </si>
+  <si>
+    <t>Search team such as volunteers, necrosearch</t>
+  </si>
+  <si>
+    <t>Photo lineup</t>
+  </si>
+  <si>
+    <t>Mitochondrial DNA</t>
+  </si>
+  <si>
+    <t>Cellphone or internet records</t>
+  </si>
+  <si>
+    <t>Toxicology</t>
+  </si>
+  <si>
+    <t>Marriage falling apart</t>
+  </si>
+  <si>
+    <t>"Life in prison"</t>
+  </si>
+  <si>
+    <t>Body found</t>
+  </si>
+  <si>
+    <t>Missing person</t>
+  </si>
+  <si>
+    <t>Body never found</t>
+  </si>
+  <si>
+    <t>Mysterious illness</t>
+  </si>
+  <si>
+    <t>Child interviewed</t>
+  </si>
+  <si>
+    <t>Items test positive for blood</t>
   </si>
 </sst>
 </file>
@@ -485,11 +533,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -725,6 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -732,6 +781,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="53.0"/>
+    <col customWidth="1" min="3" max="3" width="40.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -743,66 +793,66 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>4.0</v>
       </c>
     </row>
@@ -810,23 +860,23 @@
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>4.0</v>
       </c>
     </row>
@@ -834,31 +884,31 @@
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>4.0</v>
       </c>
     </row>
@@ -866,63 +916,63 @@
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>3.0</v>
       </c>
     </row>
@@ -930,7 +980,7 @@
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>3.0</v>
       </c>
     </row>
@@ -938,23 +988,23 @@
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>3.0</v>
       </c>
     </row>
@@ -962,255 +1012,255 @@
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>2.0</v>
       </c>
     </row>
@@ -1218,31 +1268,31 @@
       <c r="A61" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>2.0</v>
       </c>
     </row>
@@ -1250,23 +1300,23 @@
       <c r="A65" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="1">
         <v>2.0</v>
       </c>
     </row>
@@ -1274,63 +1324,63 @@
       <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -1338,55 +1388,55 @@
       <c r="A76" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -1394,111 +1444,111 @@
       <c r="A83" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="2" t="s">
+      <c r="A88" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -1506,87 +1556,87 @@
       <c r="A97" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="2" t="s">
+      <c r="A98" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B99" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="2" t="s">
+      <c r="A102" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B102" s="2">
+      <c r="B102" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="2" t="s">
+      <c r="A103" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B103" s="2">
+      <c r="B103" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="2" t="s">
+      <c r="A104" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B104" s="2">
+      <c r="B104" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="2" t="s">
+      <c r="A105" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B105" s="2">
+      <c r="B105" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="2" t="s">
+      <c r="A106" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B106" s="2">
+      <c r="B106" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="2" t="s">
+      <c r="A107" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B107" s="2">
+      <c r="B107" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -1594,127 +1644,127 @@
       <c r="A108" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B108" s="2">
+      <c r="B108" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="2" t="s">
+      <c r="A109" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B109" s="2">
+      <c r="B109" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="2" t="s">
+      <c r="A110" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B110" s="2">
+      <c r="B110" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="2" t="s">
+      <c r="A111" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B111" s="2">
+      <c r="B111" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="2" t="s">
+      <c r="A112" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B112" s="2">
+      <c r="B112" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B113" s="2">
+      <c r="B113" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="2" t="s">
+      <c r="A114" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B114" s="2">
+      <c r="B114" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B115" s="2">
+      <c r="B115" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="2" t="s">
+      <c r="A116" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B116" s="2">
+      <c r="B116" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="2" t="s">
+      <c r="A117" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B117" s="2">
+      <c r="B117" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="2" t="s">
+      <c r="A118" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B118" s="2">
+      <c r="B118" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="2" t="s">
+      <c r="A119" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B119" s="2">
+      <c r="B119" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="2" t="s">
+      <c r="A120" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B120" s="2">
+      <c r="B120" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="2" t="s">
+      <c r="A121" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B121" s="2">
+      <c r="B121" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="2" t="s">
+      <c r="A122" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B122" s="2">
+      <c r="B122" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="2" t="s">
+      <c r="A123" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B123" s="2">
+      <c r="B123" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -1722,23 +1772,23 @@
       <c r="A124" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B124" s="2">
+      <c r="B124" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="2" t="s">
+      <c r="A125" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B125" s="2">
+      <c r="B125" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="2" t="s">
+      <c r="A126" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B126" s="2">
+      <c r="B126" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -1746,47 +1796,47 @@
       <c r="A127" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B127" s="2">
+      <c r="B127" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="2" t="s">
+      <c r="A128" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B128" s="2">
+      <c r="B128" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="2" t="s">
+      <c r="A129" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B129" s="2">
+      <c r="B129" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="1" t="s">
+      <c r="A130" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B130" s="2">
+      <c r="B130" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="2" t="s">
+      <c r="A131" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B131" s="2">
+      <c r="B131" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="2" t="s">
+      <c r="A132" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B132" s="2">
+      <c r="B132" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -1794,15 +1844,15 @@
       <c r="A133" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B133" s="2">
+      <c r="B133" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="2" t="s">
+      <c r="A134" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B134" s="2">
+      <c r="B134" s="1">
         <v>4.0</v>
       </c>
     </row>
@@ -1810,12 +1860,12 @@
       <c r="A135" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B135" s="1">
-        <v>1.0</v>
+      <c r="B135" s="2">
+        <v>2.0</v>
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="2" t="s">
+      <c r="A136" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B136" s="1">
@@ -1823,42 +1873,42 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="2" t="s">
+      <c r="A137" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B137" s="2">
+      <c r="B137" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="2" t="s">
+      <c r="A138" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B138" s="2">
+      <c r="B138" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="2" t="s">
+      <c r="A139" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B139" s="2">
+      <c r="B139" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="2" t="s">
+      <c r="A140" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B140" s="2">
+      <c r="B140" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="2" t="s">
+      <c r="A141" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B141" s="2">
+      <c r="B141" s="1">
         <v>3.0</v>
       </c>
     </row>
@@ -1866,28 +1916,28 @@
       <c r="A142" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B142" s="2">
+      <c r="B142" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="2" t="s">
+      <c r="A143" s="1" t="s">
         <v>143</v>
       </c>
       <c r="B143" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="2" t="s">
+      <c r="A144" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B144" s="2">
+      <c r="B144" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="1" t="s">
+      <c r="A145" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B145" s="1">
@@ -1895,10 +1945,10 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="2" t="s">
+      <c r="A146" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B146" s="2">
+      <c r="B146" s="1">
         <v>2.0</v>
       </c>
     </row>
@@ -1906,47 +1956,47 @@
       <c r="A147" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B147" s="2">
+      <c r="B147" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="2" t="s">
+      <c r="A148" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B148" s="2">
+      <c r="B148" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="2" t="s">
+      <c r="A149" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B149" s="2">
+      <c r="B149" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="2" t="s">
+      <c r="A150" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B150" s="2">
+      <c r="B150" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="2" t="s">
+      <c r="A151" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B151" s="2">
+      <c r="B151" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="2" t="s">
+      <c r="A152" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B152" s="2">
+      <c r="B152" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -1958,7 +2008,146 @@
         <v>2.0</v>
       </c>
     </row>
+    <row r="154">
+      <c r="A154" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B154" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B155" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B156" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B157" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B158" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B159" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B160" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B161" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B162" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B163" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B164" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B165" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B166" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B167" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B168" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B169" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B170" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
   </sheetData>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="portrait" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>